<commit_message>
Additional edits to extraction names
</commit_message>
<xml_diff>
--- a/data/raw/CationExtractions_raw.xlsx
+++ b/data/raw/CationExtractions_raw.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/penninoa/Documents/VT/Data/MyData/Soil_Analyses/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nqpenelope/Documents/uvm/phd/research/data/lab/Exchangeable/VT/Soil_Analyses/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510874A5-AA67-CB40-AF9C-6E409E1B8AFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79453104-AFBB-D24A-AD98-68CE4D94F820}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="740" windowWidth="27640" windowHeight="16500" xr2:uid="{8060459B-B379-6842-8F4C-08E015D85082}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="16500" xr2:uid="{8060459B-B379-6842-8F4C-08E015D85082}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="98">
   <si>
     <t>Virginia Tech Soil Testing Laboratory</t>
   </si>
@@ -193,18 +202,6 @@
     <t>52_3_X3.1</t>
   </si>
   <si>
-    <t>BC1</t>
-  </si>
-  <si>
-    <t>BC2</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
     <t>52_2_X2.1</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>42_2_V2.1</t>
   </si>
   <si>
-    <t>E4</t>
-  </si>
-  <si>
     <t>86_3_W3.2</t>
   </si>
   <si>
@@ -238,18 +232,6 @@
     <t>Bs1</t>
   </si>
   <si>
-    <t>Bs2</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>42_4_V4.1</t>
   </si>
   <si>
@@ -262,12 +244,6 @@
     <t>Bs2.2</t>
   </si>
   <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>D9</t>
-  </si>
-  <si>
     <t>86_2_W2.1</t>
   </si>
   <si>
@@ -280,9 +256,6 @@
     <t>Bhs3.3</t>
   </si>
   <si>
-    <t>Bs3</t>
-  </si>
-  <si>
     <t>Data reported as mg/L in solution. The "-99.99" indicates concentrations less than the instrument detection limit.</t>
   </si>
   <si>
@@ -292,7 +265,70 @@
     <t>Bhs2.3</t>
   </si>
   <si>
-    <t>D10</t>
+    <t>BC.1</t>
+  </si>
+  <si>
+    <t>BC.2</t>
+  </si>
+  <si>
+    <t>D.1</t>
+  </si>
+  <si>
+    <t>D.3</t>
+  </si>
+  <si>
+    <t>E.1</t>
+  </si>
+  <si>
+    <t>E.2</t>
+  </si>
+  <si>
+    <t>E.3</t>
+  </si>
+  <si>
+    <t>E.4</t>
+  </si>
+  <si>
+    <t>D.4</t>
+  </si>
+  <si>
+    <t>D.6</t>
+  </si>
+  <si>
+    <t>D.8</t>
+  </si>
+  <si>
+    <t>D.9</t>
+  </si>
+  <si>
+    <t>D.16</t>
+  </si>
+  <si>
+    <t>BC.3</t>
+  </si>
+  <si>
+    <t>D.2</t>
+  </si>
+  <si>
+    <t>Bs.1</t>
+  </si>
+  <si>
+    <t>Bs.2</t>
+  </si>
+  <si>
+    <t>Bs.3</t>
+  </si>
+  <si>
+    <t>C.2</t>
+  </si>
+  <si>
+    <t>Bh.1</t>
+  </si>
+  <si>
+    <t>Bh.2</t>
+  </si>
+  <si>
+    <t>D.10</t>
   </si>
 </sst>
 </file>
@@ -468,6 +504,15 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
@@ -494,15 +539,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -821,15 +857,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB117DD-7230-9241-B114-EEEE02930CE9}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="10.83203125" style="14"/>
     <col min="4" max="5" width="10.83203125" style="21"/>
-    <col min="6" max="6" width="10.83203125" style="33"/>
+    <col min="6" max="6" width="10.83203125" style="24"/>
     <col min="7" max="11" width="10.83203125" style="21"/>
     <col min="12" max="16384" width="10.83203125" style="11"/>
   </cols>
@@ -850,7 +886,7 @@
       <c r="E1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="22" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="19" t="s">
@@ -880,7 +916,7 @@
       <c r="E2" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="23">
         <v>9.4E-2</v>
       </c>
       <c r="G2" s="20">
@@ -915,7 +951,7 @@
       <c r="E3" s="20">
         <v>6.8680000000000003</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="23">
         <v>0.86</v>
       </c>
       <c r="G3" s="20">
@@ -950,7 +986,7 @@
       <c r="E4" s="20">
         <v>4.2569999999999997</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="23">
         <v>0.48099999999999998</v>
       </c>
       <c r="G4" s="20">
@@ -985,7 +1021,7 @@
       <c r="E5" s="20">
         <v>4.3460000000000001</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="23">
         <v>8.3089999999999993</v>
       </c>
       <c r="G5" s="20">
@@ -1020,7 +1056,7 @@
       <c r="E6" s="20">
         <v>10.504</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="23">
         <v>1.046</v>
       </c>
       <c r="G6" s="20">
@@ -1055,7 +1091,7 @@
       <c r="E7" s="20">
         <v>2.6720000000000002</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="23">
         <v>0.93</v>
       </c>
       <c r="G7" s="20">
@@ -1090,7 +1126,7 @@
       <c r="E8" s="20">
         <v>3.073</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="23">
         <v>1.016</v>
       </c>
       <c r="G8" s="20">
@@ -1125,7 +1161,7 @@
       <c r="E9" s="20">
         <v>4.6689999999999996</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="23">
         <v>1.198</v>
       </c>
       <c r="G9" s="20">
@@ -1160,7 +1196,7 @@
       <c r="E10" s="20">
         <v>2.226</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="23">
         <v>52.545999999999999</v>
       </c>
       <c r="G10" s="20">
@@ -1195,7 +1231,7 @@
       <c r="E11" s="20">
         <v>2.5640000000000001</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="23">
         <v>3.0680000000000001</v>
       </c>
       <c r="G11" s="20">
@@ -1230,7 +1266,7 @@
       <c r="E12" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="23">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="G12" s="20">
@@ -1261,7 +1297,7 @@
       <c r="E13" s="20">
         <v>59.514000000000003</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="23">
         <v>2.4420000000000002</v>
       </c>
       <c r="G13" s="20">
@@ -1296,7 +1332,7 @@
       <c r="E14" s="20">
         <v>15.175000000000001</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="23">
         <v>1.581</v>
       </c>
       <c r="G14" s="20">
@@ -1331,7 +1367,7 @@
       <c r="E15" s="20">
         <v>1.367</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="23">
         <v>0.84099999999999997</v>
       </c>
       <c r="G15" s="20">
@@ -1366,7 +1402,7 @@
       <c r="E16" s="20">
         <v>0.55600000000000005</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="23">
         <v>0.59799999999999998</v>
       </c>
       <c r="G16" s="20">
@@ -1401,7 +1437,7 @@
       <c r="E17" s="20">
         <v>0.94799999999999995</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="23">
         <v>2.6890000000000001</v>
       </c>
       <c r="G17" s="20">
@@ -1436,7 +1472,7 @@
       <c r="E18" s="20">
         <v>0.879</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="23">
         <v>1.9470000000000001</v>
       </c>
       <c r="G18" s="20">
@@ -1471,7 +1507,7 @@
       <c r="E19" s="20">
         <v>1.1160000000000001</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="23">
         <v>1.48</v>
       </c>
       <c r="G19" s="20">
@@ -1506,7 +1542,7 @@
       <c r="E20" s="20">
         <v>8.0250000000000004</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="23">
         <v>2.3260000000000001</v>
       </c>
       <c r="G20" s="20">
@@ -1541,7 +1577,7 @@
       <c r="E21" s="20">
         <v>5.4459999999999997</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="23">
         <v>4.968</v>
       </c>
       <c r="G21" s="20">
@@ -1572,7 +1608,7 @@
       <c r="E22" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="23">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="G22" s="20">
@@ -1607,7 +1643,7 @@
       <c r="E23" s="20">
         <v>6.9509999999999996</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="23">
         <v>2.339</v>
       </c>
       <c r="G23" s="20">
@@ -1642,7 +1678,7 @@
       <c r="E24" s="20">
         <v>4.21</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="23">
         <v>1.0169999999999999</v>
       </c>
       <c r="G24" s="20">
@@ -1677,7 +1713,7 @@
       <c r="E25" s="20">
         <v>3.5219999999999998</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="23">
         <v>2.2839999999999998</v>
       </c>
       <c r="G25" s="20">
@@ -1712,7 +1748,7 @@
       <c r="E26" s="20">
         <v>1.9430000000000001</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="23">
         <v>1.5940000000000001</v>
       </c>
       <c r="G26" s="20">
@@ -1747,7 +1783,7 @@
       <c r="E27" s="20">
         <v>0.44800000000000001</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="23">
         <v>11.458</v>
       </c>
       <c r="G27" s="20">
@@ -1782,7 +1818,7 @@
       <c r="E28" s="20">
         <v>0.112</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="23">
         <v>0.41</v>
       </c>
       <c r="G28" s="20">
@@ -1817,7 +1853,7 @@
       <c r="E29" s="20">
         <v>16.87</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="23">
         <v>0.94899999999999995</v>
       </c>
       <c r="G29" s="20">
@@ -1852,7 +1888,7 @@
       <c r="E30" s="20">
         <v>0.48</v>
       </c>
-      <c r="F30" s="32">
+      <c r="F30" s="23">
         <v>0.628</v>
       </c>
       <c r="G30" s="20">
@@ -1887,7 +1923,7 @@
       <c r="E31" s="20">
         <v>0.42099999999999999</v>
       </c>
-      <c r="F31" s="32">
+      <c r="F31" s="23">
         <v>0.32200000000000001</v>
       </c>
       <c r="G31" s="20">
@@ -1922,7 +1958,7 @@
       <c r="E32" s="20">
         <v>5.0789999999999997</v>
       </c>
-      <c r="F32" s="32">
+      <c r="F32" s="23">
         <v>33.689</v>
       </c>
       <c r="G32" s="20">
@@ -1953,7 +1989,7 @@
       <c r="E33" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F33" s="32">
+      <c r="F33" s="23">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="G33" s="20">
@@ -1988,7 +2024,7 @@
       <c r="E34" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F34" s="32">
+      <c r="F34" s="23">
         <v>0.77400000000000002</v>
       </c>
       <c r="G34" s="20">
@@ -2023,7 +2059,7 @@
       <c r="E35" s="20">
         <v>1.07</v>
       </c>
-      <c r="F35" s="32">
+      <c r="F35" s="23">
         <v>6.63</v>
       </c>
       <c r="G35" s="20">
@@ -2058,7 +2094,7 @@
       <c r="E36" s="20">
         <v>1.9430000000000001</v>
       </c>
-      <c r="F36" s="32">
+      <c r="F36" s="23">
         <v>5.218</v>
       </c>
       <c r="G36" s="20">
@@ -2093,7 +2129,7 @@
       <c r="E37" s="20">
         <v>2.3319999999999999</v>
       </c>
-      <c r="F37" s="32">
+      <c r="F37" s="23">
         <v>2.4980000000000002</v>
       </c>
       <c r="G37" s="20">
@@ -2128,7 +2164,7 @@
       <c r="E38" s="20">
         <v>3.5289999999999999</v>
       </c>
-      <c r="F38" s="32">
+      <c r="F38" s="23">
         <v>0.85099999999999998</v>
       </c>
       <c r="G38" s="20">
@@ -2163,7 +2199,7 @@
       <c r="E39" s="20">
         <v>0.56899999999999995</v>
       </c>
-      <c r="F39" s="32">
+      <c r="F39" s="23">
         <v>26.905000000000001</v>
       </c>
       <c r="G39" s="20">
@@ -2198,7 +2234,7 @@
       <c r="E40" s="20">
         <v>0.38100000000000001</v>
       </c>
-      <c r="F40" s="32">
+      <c r="F40" s="23">
         <v>4.3890000000000002</v>
       </c>
       <c r="G40" s="20">
@@ -2233,7 +2269,7 @@
       <c r="E41" s="20">
         <v>39.302</v>
       </c>
-      <c r="F41" s="32">
+      <c r="F41" s="23">
         <v>8.2360000000000007</v>
       </c>
       <c r="G41" s="20">
@@ -2268,7 +2304,7 @@
       <c r="E42" s="20">
         <v>3.141</v>
       </c>
-      <c r="F42" s="32">
+      <c r="F42" s="23">
         <v>2.4710000000000001</v>
       </c>
       <c r="G42" s="20">
@@ -2303,7 +2339,7 @@
       <c r="E43" s="20">
         <v>1.72</v>
       </c>
-      <c r="F43" s="32">
+      <c r="F43" s="23">
         <v>2.7389999999999999</v>
       </c>
       <c r="G43" s="20">
@@ -2334,7 +2370,7 @@
       <c r="E44" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F44" s="32">
+      <c r="F44" s="23">
         <v>0.104</v>
       </c>
       <c r="G44" s="20">
@@ -2361,7 +2397,7 @@
         <v>51</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D45" s="20">
         <v>4.0860000000000003</v>
@@ -2369,7 +2405,7 @@
       <c r="E45" s="20">
         <v>0.88300000000000001</v>
       </c>
-      <c r="F45" s="32">
+      <c r="F45" s="23">
         <v>24.902999999999999</v>
       </c>
       <c r="G45" s="20">
@@ -2404,7 +2440,7 @@
       <c r="E46" s="20">
         <v>1.5680000000000001</v>
       </c>
-      <c r="F46" s="32">
+      <c r="F46" s="23">
         <v>6.2610000000000001</v>
       </c>
       <c r="G46" s="20">
@@ -2439,7 +2475,7 @@
       <c r="E47" s="20">
         <v>1.9690000000000001</v>
       </c>
-      <c r="F47" s="32">
+      <c r="F47" s="23">
         <v>5.7919999999999998</v>
       </c>
       <c r="G47" s="20">
@@ -2474,7 +2510,7 @@
       <c r="E48" s="20">
         <v>1.1759999999999999</v>
       </c>
-      <c r="F48" s="32">
+      <c r="F48" s="23">
         <v>3.0339999999999998</v>
       </c>
       <c r="G48" s="20">
@@ -2509,7 +2545,7 @@
       <c r="E49" s="20">
         <v>1.92</v>
       </c>
-      <c r="F49" s="32">
+      <c r="F49" s="23">
         <v>7.53</v>
       </c>
       <c r="G49" s="20">
@@ -2544,7 +2580,7 @@
       <c r="E50" s="20">
         <v>2.1789999999999998</v>
       </c>
-      <c r="F50" s="32">
+      <c r="F50" s="23">
         <v>0.84799999999999998</v>
       </c>
       <c r="G50" s="20">
@@ -2579,7 +2615,7 @@
       <c r="E51" s="20">
         <v>25.356999999999999</v>
       </c>
-      <c r="F51" s="32">
+      <c r="F51" s="23">
         <v>1.8680000000000001</v>
       </c>
       <c r="G51" s="20">
@@ -2614,7 +2650,7 @@
       <c r="E52" s="20">
         <v>13.01</v>
       </c>
-      <c r="F52" s="32">
+      <c r="F52" s="23">
         <v>1.6850000000000001</v>
       </c>
       <c r="G52" s="20">
@@ -2649,7 +2685,7 @@
       <c r="E53" s="20">
         <v>4.7290000000000001</v>
       </c>
-      <c r="F53" s="32">
+      <c r="F53" s="23">
         <v>1.034</v>
       </c>
       <c r="G53" s="20">
@@ -2676,7 +2712,7 @@
         <v>54</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D54" s="20">
         <v>-99.99</v>
@@ -2684,7 +2720,7 @@
       <c r="E54" s="20">
         <v>2.7530000000000001</v>
       </c>
-      <c r="F54" s="32">
+      <c r="F54" s="23">
         <v>1.2310000000000001</v>
       </c>
       <c r="G54" s="20">
@@ -2715,7 +2751,7 @@
       <c r="E55" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F55" s="32">
+      <c r="F55" s="23">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="G55" s="20">
@@ -2742,7 +2778,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D56" s="20">
         <v>-99.99</v>
@@ -2750,7 +2786,7 @@
       <c r="E56" s="20">
         <v>0.80200000000000005</v>
       </c>
-      <c r="F56" s="32">
+      <c r="F56" s="23">
         <v>0.77900000000000003</v>
       </c>
       <c r="G56" s="20">
@@ -2777,7 +2813,7 @@
         <v>54</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D57" s="20">
         <v>-99.99</v>
@@ -2785,7 +2821,7 @@
       <c r="E57" s="20">
         <v>0.68400000000000005</v>
       </c>
-      <c r="F57" s="32">
+      <c r="F57" s="23">
         <v>0.49099999999999999</v>
       </c>
       <c r="G57" s="20">
@@ -2812,7 +2848,7 @@
         <v>54</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D58" s="20">
         <v>0.88900000000000001</v>
@@ -2820,7 +2856,7 @@
       <c r="E58" s="20">
         <v>3.427</v>
       </c>
-      <c r="F58" s="32">
+      <c r="F58" s="23">
         <v>8.0649999999999995</v>
       </c>
       <c r="G58" s="20">
@@ -2847,7 +2883,7 @@
         <v>54</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="D59" s="20">
         <v>-99.99</v>
@@ -2855,7 +2891,7 @@
       <c r="E59" s="20">
         <v>0.93500000000000005</v>
       </c>
-      <c r="F59" s="32">
+      <c r="F59" s="23">
         <v>4.6719999999999997</v>
       </c>
       <c r="G59" s="20">
@@ -2879,10 +2915,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D60" s="20">
         <v>-99.99</v>
@@ -2890,7 +2926,7 @@
       <c r="E60" s="20">
         <v>3.7450000000000001</v>
       </c>
-      <c r="F60" s="32">
+      <c r="F60" s="23">
         <v>0.80800000000000005</v>
       </c>
       <c r="G60" s="20">
@@ -2914,10 +2950,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D61" s="20">
         <v>-99.99</v>
@@ -2925,7 +2961,7 @@
       <c r="E61" s="20">
         <v>3.1440000000000001</v>
       </c>
-      <c r="F61" s="32">
+      <c r="F61" s="23">
         <v>0.68300000000000005</v>
       </c>
       <c r="G61" s="20">
@@ -2949,7 +2985,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C62" s="17" t="s">
         <v>27</v>
@@ -2960,7 +2996,7 @@
       <c r="E62" s="20">
         <v>2.1539999999999999</v>
       </c>
-      <c r="F62" s="32">
+      <c r="F62" s="23">
         <v>0.49199999999999999</v>
       </c>
       <c r="G62" s="20">
@@ -2984,7 +3020,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C63" s="17" t="s">
         <v>29</v>
@@ -2995,7 +3031,7 @@
       <c r="E63" s="20">
         <v>7.7380000000000004</v>
       </c>
-      <c r="F63" s="32">
+      <c r="F63" s="23">
         <v>8.0640000000000001</v>
       </c>
       <c r="G63" s="20">
@@ -3019,10 +3055,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="D64" s="20">
         <v>2.3079999999999998</v>
@@ -3030,7 +3066,7 @@
       <c r="E64" s="20">
         <v>2.6219999999999999</v>
       </c>
-      <c r="F64" s="32">
+      <c r="F64" s="23">
         <v>0.99</v>
       </c>
       <c r="G64" s="20">
@@ -3061,7 +3097,7 @@
       <c r="E65" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F65" s="32">
+      <c r="F65" s="23">
         <v>-99.99</v>
       </c>
       <c r="G65" s="20">
@@ -3085,10 +3121,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="D66" s="20">
         <v>-99.99</v>
@@ -3096,7 +3132,7 @@
       <c r="E66" s="20">
         <v>2.702</v>
       </c>
-      <c r="F66" s="32">
+      <c r="F66" s="23">
         <v>0.436</v>
       </c>
       <c r="G66" s="20">
@@ -3120,10 +3156,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D67" s="20">
         <v>0.13100000000000001</v>
@@ -3131,7 +3167,7 @@
       <c r="E67" s="20">
         <v>5.32</v>
       </c>
-      <c r="F67" s="32">
+      <c r="F67" s="23">
         <v>0.39400000000000002</v>
       </c>
       <c r="G67" s="20">
@@ -3155,10 +3191,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="D68" s="20">
         <v>-99.99</v>
@@ -3166,7 +3202,7 @@
       <c r="E68" s="20">
         <v>4.3570000000000002</v>
       </c>
-      <c r="F68" s="32">
+      <c r="F68" s="23">
         <v>0.39600000000000002</v>
       </c>
       <c r="G68" s="20">
@@ -3190,7 +3226,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C69" s="17" t="s">
         <v>29</v>
@@ -3201,7 +3237,7 @@
       <c r="E69" s="20">
         <v>0.85399999999999998</v>
       </c>
-      <c r="F69" s="32">
+      <c r="F69" s="23">
         <v>59.976999999999997</v>
       </c>
       <c r="G69" s="20">
@@ -3225,10 +3261,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D70" s="20">
         <v>-99.99</v>
@@ -3236,7 +3272,7 @@
       <c r="E70" s="20">
         <v>22.393000000000001</v>
       </c>
-      <c r="F70" s="32">
+      <c r="F70" s="23">
         <v>8.8109999999999999</v>
       </c>
       <c r="G70" s="20">
@@ -3260,7 +3296,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C71" s="17" t="s">
         <v>30</v>
@@ -3271,7 +3307,7 @@
       <c r="E71" s="20">
         <v>32.466000000000001</v>
       </c>
-      <c r="F71" s="32">
+      <c r="F71" s="23">
         <v>4.0140000000000002</v>
       </c>
       <c r="G71" s="20">
@@ -3295,7 +3331,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C72" s="17" t="s">
         <v>52</v>
@@ -3306,7 +3342,7 @@
       <c r="E72" s="20">
         <v>18.811</v>
       </c>
-      <c r="F72" s="32">
+      <c r="F72" s="23">
         <v>2.5470000000000002</v>
       </c>
       <c r="G72" s="20">
@@ -3330,7 +3366,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C73" s="17" t="s">
         <v>53</v>
@@ -3341,7 +3377,7 @@
       <c r="E73" s="20">
         <v>40.426000000000002</v>
       </c>
-      <c r="F73" s="32">
+      <c r="F73" s="23">
         <v>3.09</v>
       </c>
       <c r="G73" s="20">
@@ -3365,10 +3401,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D74" s="20">
         <v>-99.99</v>
@@ -3376,7 +3412,7 @@
       <c r="E74" s="20">
         <v>26.51</v>
       </c>
-      <c r="F74" s="32">
+      <c r="F74" s="23">
         <v>1.502</v>
       </c>
       <c r="G74" s="20">
@@ -3400,10 +3436,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D75" s="20">
         <v>-99.99</v>
@@ -3411,7 +3447,7 @@
       <c r="E75" s="20">
         <v>29.1</v>
       </c>
-      <c r="F75" s="32">
+      <c r="F75" s="23">
         <v>1.5149999999999999</v>
       </c>
       <c r="G75" s="20">
@@ -3442,7 +3478,7 @@
       <c r="E76" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F76" s="32">
+      <c r="F76" s="23">
         <v>-99.99</v>
       </c>
       <c r="G76" s="20">
@@ -3466,7 +3502,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C77" s="17" t="s">
         <v>29</v>
@@ -3477,7 +3513,7 @@
       <c r="E77" s="20">
         <v>0.88100000000000001</v>
       </c>
-      <c r="F77" s="32">
+      <c r="F77" s="23">
         <v>85.885999999999996</v>
       </c>
       <c r="G77" s="20">
@@ -3501,7 +3537,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C78" s="17" t="s">
         <v>35</v>
@@ -3512,7 +3548,7 @@
       <c r="E78" s="20">
         <v>1.083</v>
       </c>
-      <c r="F78" s="32">
+      <c r="F78" s="23">
         <v>4.1420000000000003</v>
       </c>
       <c r="G78" s="20">
@@ -3536,7 +3572,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>38</v>
@@ -3547,7 +3583,7 @@
       <c r="E79" s="20">
         <v>55.421999999999997</v>
       </c>
-      <c r="F79" s="32">
+      <c r="F79" s="23">
         <v>9.4090000000000007</v>
       </c>
       <c r="G79" s="20">
@@ -3571,10 +3607,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="D80" s="20">
         <v>-99.99</v>
@@ -3582,7 +3618,7 @@
       <c r="E80" s="20">
         <v>19.456</v>
       </c>
-      <c r="F80" s="32">
+      <c r="F80" s="23">
         <v>2.1619999999999999</v>
       </c>
       <c r="G80" s="20">
@@ -3606,10 +3642,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D81" s="20">
         <v>-99.99</v>
@@ -3617,7 +3653,7 @@
       <c r="E81" s="20">
         <v>8.6199999999999992</v>
       </c>
-      <c r="F81" s="32">
+      <c r="F81" s="23">
         <v>1.859</v>
       </c>
       <c r="G81" s="20">
@@ -3641,10 +3677,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D82" s="20">
         <v>-99.99</v>
@@ -3652,7 +3688,7 @@
       <c r="E82" s="20">
         <v>6.6040000000000001</v>
       </c>
-      <c r="F82" s="32">
+      <c r="F82" s="23">
         <v>1.4339999999999999</v>
       </c>
       <c r="G82" s="20">
@@ -3676,10 +3712,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D83" s="20">
         <v>-99.99</v>
@@ -3687,7 +3723,7 @@
       <c r="E83" s="20">
         <v>1.7310000000000001</v>
       </c>
-      <c r="F83" s="32">
+      <c r="F83" s="23">
         <v>1.141</v>
       </c>
       <c r="G83" s="20">
@@ -3711,10 +3747,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D84" s="20">
         <v>-99.99</v>
@@ -3722,7 +3758,7 @@
       <c r="E84" s="20">
         <v>4.0469999999999997</v>
       </c>
-      <c r="F84" s="32">
+      <c r="F84" s="23">
         <v>1.1140000000000001</v>
       </c>
       <c r="G84" s="20">
@@ -3746,10 +3782,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="D85" s="20">
         <v>-99.99</v>
@@ -3757,7 +3793,7 @@
       <c r="E85" s="20">
         <v>4.2960000000000003</v>
       </c>
-      <c r="F85" s="32">
+      <c r="F85" s="23">
         <v>1.4630000000000001</v>
       </c>
       <c r="G85" s="20">
@@ -3781,10 +3817,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D86" s="20">
         <v>-99.99</v>
@@ -3792,7 +3828,7 @@
       <c r="E86" s="20">
         <v>3.9089999999999998</v>
       </c>
-      <c r="F86" s="32">
+      <c r="F86" s="23">
         <v>0.69699999999999995</v>
       </c>
       <c r="G86" s="20">
@@ -3823,7 +3859,7 @@
       <c r="E87" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F87" s="32">
+      <c r="F87" s="23">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="G87" s="20">
@@ -3847,7 +3883,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C88" s="17" t="s">
         <v>29</v>
@@ -3858,7 +3894,7 @@
       <c r="E88" s="20">
         <v>1.125</v>
       </c>
-      <c r="F88" s="32">
+      <c r="F88" s="23">
         <v>50.171999999999997</v>
       </c>
       <c r="G88" s="20">
@@ -3882,7 +3918,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C89" s="17" t="s">
         <v>35</v>
@@ -3893,7 +3929,7 @@
       <c r="E89" s="20">
         <v>1.1240000000000001</v>
       </c>
-      <c r="F89" s="32">
+      <c r="F89" s="23">
         <v>2.0369999999999999</v>
       </c>
       <c r="G89" s="20">
@@ -3917,7 +3953,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C90" s="17" t="s">
         <v>30</v>
@@ -3928,7 +3964,7 @@
       <c r="E90" s="20">
         <v>14.509</v>
       </c>
-      <c r="F90" s="32">
+      <c r="F90" s="23">
         <v>2.99</v>
       </c>
       <c r="G90" s="20">
@@ -3952,7 +3988,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C91" s="13" t="s">
         <v>52</v>
@@ -3963,7 +3999,7 @@
       <c r="E91" s="20">
         <v>15.773999999999999</v>
       </c>
-      <c r="F91" s="32">
+      <c r="F91" s="23">
         <v>2.8690000000000002</v>
       </c>
       <c r="G91" s="20">
@@ -3987,7 +4023,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C92" s="13" t="s">
         <v>53</v>
@@ -3998,7 +4034,7 @@
       <c r="E92" s="20">
         <v>11.94</v>
       </c>
-      <c r="F92" s="32">
+      <c r="F92" s="23">
         <v>2.6080000000000001</v>
       </c>
       <c r="G92" s="20">
@@ -4022,10 +4058,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="D93" s="20">
         <v>-99.99</v>
@@ -4033,7 +4069,7 @@
       <c r="E93" s="20">
         <v>4.556</v>
       </c>
-      <c r="F93" s="32">
+      <c r="F93" s="23">
         <v>1.714</v>
       </c>
       <c r="G93" s="20">
@@ -4057,10 +4093,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D94" s="20">
         <v>-99.99</v>
@@ -4068,7 +4104,7 @@
       <c r="E94" s="20">
         <v>1.7869999999999999</v>
       </c>
-      <c r="F94" s="32">
+      <c r="F94" s="23">
         <v>1.0229999999999999</v>
       </c>
       <c r="G94" s="20">
@@ -4092,7 +4128,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C95" s="13" t="s">
         <v>33</v>
@@ -4103,7 +4139,7 @@
       <c r="E95" s="20">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F95" s="32">
+      <c r="F95" s="23">
         <v>0.7</v>
       </c>
       <c r="G95" s="20">
@@ -4127,10 +4163,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="D96" s="20">
         <v>-99.99</v>
@@ -4138,7 +4174,7 @@
       <c r="E96" s="20">
         <v>0.52800000000000002</v>
       </c>
-      <c r="F96" s="32">
+      <c r="F96" s="23">
         <v>0.36899999999999999</v>
       </c>
       <c r="G96" s="20">
@@ -4162,10 +4198,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D97" s="20">
         <v>-99.99</v>
@@ -4173,7 +4209,7 @@
       <c r="E97" s="20">
         <v>1.8520000000000001</v>
       </c>
-      <c r="F97" s="32">
+      <c r="F97" s="23">
         <v>0.76</v>
       </c>
       <c r="G97" s="20">
@@ -4204,7 +4240,7 @@
       <c r="E98" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F98" s="32">
+      <c r="F98" s="23">
         <v>-99.99</v>
       </c>
       <c r="G98" s="20">
@@ -4228,7 +4264,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C99" s="17" t="s">
         <v>29</v>
@@ -4239,7 +4275,7 @@
       <c r="E99" s="20">
         <v>1.2589999999999999</v>
       </c>
-      <c r="F99" s="32">
+      <c r="F99" s="23">
         <v>3.3119999999999998</v>
       </c>
       <c r="G99" s="20">
@@ -4263,7 +4299,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C100" s="17" t="s">
         <v>35</v>
@@ -4274,7 +4310,7 @@
       <c r="E100" s="20">
         <v>1.7669999999999999</v>
       </c>
-      <c r="F100" s="32">
+      <c r="F100" s="23">
         <v>0.61599999999999999</v>
       </c>
       <c r="G100" s="20">
@@ -4298,7 +4334,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C101" s="17" t="s">
         <v>38</v>
@@ -4309,7 +4345,7 @@
       <c r="E101" s="20">
         <v>12.379</v>
       </c>
-      <c r="F101" s="32">
+      <c r="F101" s="23">
         <v>1.171</v>
       </c>
       <c r="G101" s="20">
@@ -4333,10 +4369,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D102" s="20">
         <v>-99.99</v>
@@ -4344,7 +4380,7 @@
       <c r="E102" s="20">
         <v>6.4660000000000002</v>
       </c>
-      <c r="F102" s="32">
+      <c r="F102" s="23">
         <v>1.177</v>
       </c>
       <c r="G102" s="20">
@@ -4368,10 +4404,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D103" s="20">
         <v>-99.99</v>
@@ -4379,7 +4415,7 @@
       <c r="E103" s="20">
         <v>1.454</v>
       </c>
-      <c r="F103" s="32">
+      <c r="F103" s="23">
         <v>1.425</v>
       </c>
       <c r="G103" s="20">
@@ -4403,10 +4439,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D104" s="20">
         <v>-99.99</v>
@@ -4414,7 +4450,7 @@
       <c r="E104" s="20">
         <v>1.006</v>
       </c>
-      <c r="F104" s="32">
+      <c r="F104" s="23">
         <v>1.038</v>
       </c>
       <c r="G104" s="20">
@@ -4438,10 +4474,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D105" s="20">
         <v>-99.99</v>
@@ -4449,7 +4485,7 @@
       <c r="E105" s="20">
         <v>0.64600000000000002</v>
       </c>
-      <c r="F105" s="32">
+      <c r="F105" s="23">
         <v>0.60899999999999999</v>
       </c>
       <c r="G105" s="20">
@@ -4473,10 +4509,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D106" s="20">
         <v>-99.99</v>
@@ -4484,7 +4520,7 @@
       <c r="E106" s="20">
         <v>0.99099999999999999</v>
       </c>
-      <c r="F106" s="32">
+      <c r="F106" s="23">
         <v>0.61199999999999999</v>
       </c>
       <c r="G106" s="20">
@@ -4508,10 +4544,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="D107" s="20">
         <v>-99.99</v>
@@ -4519,7 +4555,7 @@
       <c r="E107" s="20">
         <v>0.64900000000000002</v>
       </c>
-      <c r="F107" s="32">
+      <c r="F107" s="23">
         <v>0.53800000000000003</v>
       </c>
       <c r="G107" s="20">
@@ -4543,10 +4579,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D108" s="20">
         <v>-99.99</v>
@@ -4554,7 +4590,7 @@
       <c r="E108" s="20">
         <v>7.7320000000000002</v>
       </c>
-      <c r="F108" s="32">
+      <c r="F108" s="23">
         <v>0.82499999999999996</v>
       </c>
       <c r="G108" s="20">
@@ -4585,7 +4621,7 @@
       <c r="E109" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F109" s="32">
+      <c r="F109" s="23">
         <v>-99.99</v>
       </c>
       <c r="G109" s="20">
@@ -4609,10 +4645,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D110" s="20">
         <v>-99.99</v>
@@ -4620,7 +4656,7 @@
       <c r="E110" s="20">
         <v>0.65200000000000002</v>
       </c>
-      <c r="F110" s="32">
+      <c r="F110" s="23">
         <v>0.47499999999999998</v>
       </c>
       <c r="G110" s="20">
@@ -4644,10 +4680,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D111" s="20">
         <v>-99.99</v>
@@ -4655,7 +4691,7 @@
       <c r="E111" s="20">
         <v>0.53400000000000003</v>
       </c>
-      <c r="F111" s="32">
+      <c r="F111" s="23">
         <v>0.54800000000000004</v>
       </c>
       <c r="G111" s="20">
@@ -4679,10 +4715,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="D112" s="20">
         <v>-99.99</v>
@@ -4690,7 +4726,7 @@
       <c r="E112" s="20">
         <v>0.47499999999999998</v>
       </c>
-      <c r="F112" s="32">
+      <c r="F112" s="23">
         <v>17.827000000000002</v>
       </c>
       <c r="G112" s="20">
@@ -4714,10 +4750,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C113" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="C113" s="17" t="s">
-        <v>26</v>
       </c>
       <c r="D113" s="20">
         <v>-99.99</v>
@@ -4725,7 +4761,7 @@
       <c r="E113" s="20">
         <v>2.452</v>
       </c>
-      <c r="F113" s="32">
+      <c r="F113" s="23">
         <v>2.4750000000000001</v>
       </c>
       <c r="G113" s="20">
@@ -4749,10 +4785,10 @@
         <v>113</v>
       </c>
       <c r="B114" s="17" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="D114" s="20">
         <v>-99.99</v>
@@ -4760,7 +4796,7 @@
       <c r="E114" s="20">
         <v>2.65</v>
       </c>
-      <c r="F114" s="32">
+      <c r="F114" s="23">
         <v>4.0090000000000003</v>
       </c>
       <c r="G114" s="20">
@@ -4784,7 +4820,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C115" s="17" t="s">
         <v>30</v>
@@ -4795,7 +4831,7 @@
       <c r="E115" s="20">
         <v>2.089</v>
       </c>
-      <c r="F115" s="32">
+      <c r="F115" s="23">
         <v>0.63200000000000001</v>
       </c>
       <c r="G115" s="20">
@@ -4819,7 +4855,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C116" s="17" t="s">
         <v>52</v>
@@ -4830,7 +4866,7 @@
       <c r="E116" s="20">
         <v>2.7</v>
       </c>
-      <c r="F116" s="32">
+      <c r="F116" s="23">
         <v>0.86799999999999999</v>
       </c>
       <c r="G116" s="20">
@@ -4854,7 +4890,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C117" s="17" t="s">
         <v>53</v>
@@ -4865,7 +4901,7 @@
       <c r="E117" s="20">
         <v>1.9670000000000001</v>
       </c>
-      <c r="F117" s="32">
+      <c r="F117" s="23">
         <v>1.0609999999999999</v>
       </c>
       <c r="G117" s="20">
@@ -4896,7 +4932,7 @@
       <c r="E118" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F118" s="32">
+      <c r="F118" s="23">
         <v>-99.99</v>
       </c>
       <c r="G118" s="20">
@@ -4920,10 +4956,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D119" s="20">
         <v>0.90300000000000002</v>
@@ -4931,7 +4967,7 @@
       <c r="E119" s="20">
         <v>2.1429999999999998</v>
       </c>
-      <c r="F119" s="32">
+      <c r="F119" s="23">
         <v>0.89800000000000002</v>
       </c>
       <c r="G119" s="20">
@@ -4955,10 +4991,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D120" s="20">
         <v>0.36499999999999999</v>
@@ -4966,7 +5002,7 @@
       <c r="E120" s="20">
         <v>1.5229999999999999</v>
       </c>
-      <c r="F120" s="32">
+      <c r="F120" s="23">
         <v>0.78400000000000003</v>
       </c>
       <c r="G120" s="20">
@@ -4990,10 +5026,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D121" s="20">
         <v>-99.99</v>
@@ -5001,7 +5037,7 @@
       <c r="E121" s="20">
         <v>1.62</v>
       </c>
-      <c r="F121" s="32">
+      <c r="F121" s="23">
         <v>0.65700000000000003</v>
       </c>
       <c r="G121" s="20">
@@ -5025,10 +5061,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D122" s="20">
         <v>-99.99</v>
@@ -5036,7 +5072,7 @@
       <c r="E122" s="20">
         <v>1.351</v>
       </c>
-      <c r="F122" s="32">
+      <c r="F122" s="23">
         <v>0.59799999999999998</v>
       </c>
       <c r="G122" s="20">
@@ -5060,10 +5096,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D123" s="20">
         <v>-99.99</v>
@@ -5071,7 +5107,7 @@
       <c r="E123" s="20">
         <v>0.98699999999999999</v>
       </c>
-      <c r="F123" s="32">
+      <c r="F123" s="23">
         <v>0.56999999999999995</v>
       </c>
       <c r="G123" s="20">
@@ -5095,10 +5131,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C124" s="13" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D124" s="20">
         <v>-99.99</v>
@@ -5106,7 +5142,7 @@
       <c r="E124" s="20">
         <v>0.70699999999999996</v>
       </c>
-      <c r="F124" s="32">
+      <c r="F124" s="23">
         <v>0.41099999999999998</v>
       </c>
       <c r="G124" s="20">
@@ -5130,10 +5166,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D125" s="20">
         <v>-99.99</v>
@@ -5141,7 +5177,7 @@
       <c r="E125" s="20">
         <v>0.79600000000000004</v>
       </c>
-      <c r="F125" s="32">
+      <c r="F125" s="23">
         <v>0.40500000000000003</v>
       </c>
       <c r="G125" s="20">
@@ -5165,10 +5201,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="17" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D126" s="20">
         <v>0.23799999999999999</v>
@@ -5176,7 +5212,7 @@
       <c r="E126" s="20">
         <v>1.873</v>
       </c>
-      <c r="F126" s="32">
+      <c r="F126" s="23">
         <v>1.018</v>
       </c>
       <c r="G126" s="20">
@@ -5200,7 +5236,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="17" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C127" s="17" t="s">
         <v>29</v>
@@ -5211,7 +5247,7 @@
       <c r="E127" s="20">
         <v>0.14099999999999999</v>
       </c>
-      <c r="F127" s="32">
+      <c r="F127" s="23">
         <v>54.841999999999999</v>
       </c>
       <c r="G127" s="20">
@@ -5235,10 +5271,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="17" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C128" s="17" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="D128" s="20">
         <v>-99.99</v>
@@ -5246,7 +5282,7 @@
       <c r="E128" s="20">
         <v>0.245</v>
       </c>
-      <c r="F128" s="32">
+      <c r="F128" s="23">
         <v>0.59099999999999997</v>
       </c>
       <c r="G128" s="20">
@@ -5277,7 +5313,7 @@
       <c r="E129" s="20">
         <v>-99.99</v>
       </c>
-      <c r="F129" s="32">
+      <c r="F129" s="23">
         <v>-99.99</v>
       </c>
       <c r="G129" s="20">
@@ -5301,10 +5337,10 @@
         <v>129</v>
       </c>
       <c r="B130" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C130" s="17" t="s">
         <v>81</v>
-      </c>
-      <c r="C130" s="17" t="s">
-        <v>27</v>
       </c>
       <c r="D130" s="20">
         <v>-99.99</v>
@@ -5312,7 +5348,7 @@
       <c r="E130" s="20">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F130" s="32">
+      <c r="F130" s="23">
         <v>0.69799999999999995</v>
       </c>
       <c r="G130" s="20">
@@ -5336,10 +5372,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C131" s="17" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D131" s="20">
         <v>-99.99</v>
@@ -5347,7 +5383,7 @@
       <c r="E131" s="20">
         <v>1.4330000000000001</v>
       </c>
-      <c r="F131" s="32">
+      <c r="F131" s="23">
         <v>1.712</v>
       </c>
       <c r="G131" s="20">
@@ -5382,7 +5418,7 @@
       <c r="E132" s="20">
         <v>5.27</v>
       </c>
-      <c r="F132" s="32">
+      <c r="F132" s="23">
         <v>4.944</v>
       </c>
       <c r="G132" s="20">
@@ -5415,7 +5451,7 @@
       <c r="E133" s="20">
         <v>6.2480000000000002</v>
       </c>
-      <c r="F133" s="32">
+      <c r="F133" s="23">
         <v>1.1499999999999999</v>
       </c>
       <c r="G133" s="20">
@@ -5450,40 +5486,40 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -5499,11 +5535,11 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="2"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -5513,11 +5549,11 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -5527,11 +5563,11 @@
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="25">
         <v>5593</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -5541,11 +5577,11 @@
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="29">
         <v>44301</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -5555,11 +5591,11 @@
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="29">
         <v>44306</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -5569,11 +5605,11 @@
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -5583,11 +5619,11 @@
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="32">
         <v>1457.28</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -5604,15 +5640,15 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
+      <c r="A13" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New script for new ICP data
processed new ICP data, separated new script incorporating changes
</commit_message>
<xml_diff>
--- a/data/raw/CationExtractions_raw.xlsx
+++ b/data/raw/CationExtractions_raw.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nqpenelope/Documents/uvm/phd/research/data/lab/Exchangeable/VT/Soil_Analyses/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79453104-AFBB-D24A-AD98-68CE4D94F820}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B67ECB-8038-4A49-AC56-1AD793D55755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="16500" xr2:uid="{8060459B-B379-6842-8F4C-08E015D85082}"/>
+    <workbookView xWindow="-1260" yWindow="500" windowWidth="27640" windowHeight="16500" xr2:uid="{8060459B-B379-6842-8F4C-08E015D85082}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$K$133</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -420,12 +423,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -441,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,18 +522,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -539,6 +536,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -857,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB117DD-7230-9241-B114-EEEE02930CE9}">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="182" workbookViewId="0">
+      <selection activeCell="C71" sqref="B71:C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1250,69 +1271,69 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
+    <row r="12" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34">
         <v>11</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="20">
-        <v>-99.99</v>
-      </c>
-      <c r="E12" s="20">
-        <v>-99.99</v>
-      </c>
-      <c r="F12" s="23">
+      <c r="D12" s="36">
+        <v>-99.99</v>
+      </c>
+      <c r="E12" s="36">
+        <v>-99.99</v>
+      </c>
+      <c r="F12" s="36">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="G12" s="20">
-        <v>-99.99</v>
-      </c>
-      <c r="H12" s="20">
+      <c r="G12" s="36">
+        <v>-99.99</v>
+      </c>
+      <c r="H12" s="36">
         <v>0.114</v>
       </c>
-      <c r="I12" s="20">
-        <v>-99.99</v>
-      </c>
-      <c r="J12" s="20">
+      <c r="I12" s="36">
+        <v>-99.99</v>
+      </c>
+      <c r="J12" s="36">
         <v>0.315</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="36">
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="20">
-        <v>-99.99</v>
-      </c>
-      <c r="E13" s="20">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="36">
+        <v>-99.99</v>
+      </c>
+      <c r="E13" s="36">
         <v>59.514000000000003</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="36">
         <v>2.4420000000000002</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="36">
         <v>7.5609999999999999</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="36">
         <v>1.069</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="36">
         <v>1.3080000000000001</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="36">
         <v>2.0760000000000001</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13" s="36">
         <v>3.6459999999999999</v>
       </c>
     </row>
@@ -5471,6 +5492,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K133" xr:uid="{758AD3DA-FFF5-104D-8CB2-0C7A50C6CB47}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5486,40 +5508,40 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -5535,11 +5557,11 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="2"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -5549,11 +5571,11 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -5563,11 +5585,11 @@
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="30">
         <v>5593</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -5577,11 +5599,11 @@
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="25">
         <v>44301</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -5591,11 +5613,11 @@
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="25">
         <v>44306</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -5605,11 +5627,11 @@
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -5619,11 +5641,11 @@
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="28">
         <v>1457.28</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -5640,30 +5662,30 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A13:G13"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A13:G13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{A9470342-9082-6945-8C44-D1267B4B0C49}"/>

</xml_diff>